<commit_message>
Update solution-template and IDP with content constraints and multi-sheet config
Solution Template:
- Update closeout-presentation.md with content limits (5-6 items per two-column section)
- Update project-plan.csv milestone column widths (14, 20)
- Regenerate all Office documents

AWS IDP Solution:
- Fix configuration.csv: remove Bedrock/SageMaker, add A2I parameters
- Update closeout-presentation.md with content constraints
- Update project-plan.csv milestone column widths
- Regenerate all Office documents with multi-sheet configuration
- Remove deprecated artifacts (communication-plan, requirements, roles, training-plan)
</commit_message>
<xml_diff>
--- a/solution-template/sample-provider/sample-category/sample-solution/delivery/project-plan.xlsx
+++ b/solution-template/sample-provider/sample-category/sample-solution/delivery/project-plan.xlsx
@@ -2031,9 +2031,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
     <col width="77" customWidth="1" min="4" max="4"/>
     <col width="28" customWidth="1" min="5" max="5"/>
     <col width="17" customWidth="1" min="6" max="6"/>

</xml_diff>